<commit_message>
More flaming updated transfer spreadsheet template
</commit_message>
<xml_diff>
--- a/ui/app/static/transfer_template.xlsx
+++ b/ui/app/static/transfer_template.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="166">
   <si>
     <t>Remarks</t>
   </si>
@@ -555,6 +555,30 @@
   </si>
   <si>
     <t>Folder -</t>
+  </si>
+  <si>
+    <t>Photographic - Print</t>
+  </si>
+  <si>
+    <t>Photographic - Negative</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Transparency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Glass Plate Negative </t>
+  </si>
+  <si>
+    <t>Photographic - Slide</t>
+  </si>
+  <si>
+    <t>Folder</t>
+  </si>
+  <si>
+    <t>Digital media - Optical - CD</t>
+  </si>
+  <si>
+    <t>Digital media - Optical - DVD</t>
   </si>
 </sst>
 </file>
@@ -734,8 +758,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -890,9 +922,17 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1508,7 +1548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3213,8 +3253,8 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3492,7 +3532,7 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>114</v>
@@ -3505,7 +3545,7 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="12" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>75</v>
@@ -3518,7 +3558,7 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="12" t="s">
-        <v>93</v>
+        <v>160</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>115</v>
@@ -3531,7 +3571,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="12" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>64</v>
@@ -3544,10 +3584,10 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="12" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>61</v>
+        <v>163</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -3683,7 +3723,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10" t="s">
-        <v>66</v>
+        <v>164</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -3694,7 +3734,7 @@
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="G34" s="10"/>
     </row>
@@ -3755,6 +3795,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <tableParts count="7">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Fixed example sheet for fixed vocabularies
</commit_message>
<xml_diff>
--- a/ui/app/static/transfer_template.xlsx
+++ b/ui/app/static/transfer_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="26929"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="832"/>
+    <workbookView xWindow="220" yWindow="240" windowWidth="25600" windowHeight="16060" tabRatio="832"/>
   </bookViews>
   <sheets>
     <sheet name=" Transfer List Template w e.g." sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="165">
   <si>
     <t>Remarks</t>
   </si>
@@ -222,9 +222,6 @@
   </si>
   <si>
     <t>Box - Type 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Folder - </t>
   </si>
   <si>
     <t>Folder - Map</t>
@@ -758,8 +755,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -922,17 +923,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="15">
@@ -1548,7 +1553,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1559,8 +1564,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1500" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="2260" activePane="bottomLeft"/>
       <selection activeCell="V1" sqref="V1"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1613,22 +1618,22 @@
         <v>13</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I1" s="24" t="s">
         <v>49</v>
       </c>
       <c r="J1" s="50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K1" s="24" t="s">
         <v>50</v>
       </c>
       <c r="L1" s="50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M1" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="N1" s="31" t="s">
         <v>15</v>
@@ -1652,7 +1657,7 @@
         <v>4</v>
       </c>
       <c r="U1" s="40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="V1" s="24" t="s">
         <v>0</v>
@@ -1660,34 +1665,34 @@
     </row>
     <row r="2" spans="1:22" s="20" customFormat="1" ht="70">
       <c r="B2" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D2" s="20">
         <v>1</v>
       </c>
       <c r="F2" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H2" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K2" s="41">
         <v>10866</v>
       </c>
       <c r="L2" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M2" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N2" s="20">
         <v>30</v>
@@ -1696,7 +1701,7 @@
         <v>29</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="20" t="s">
         <v>32</v>
@@ -1713,26 +1718,26 @@
     </row>
     <row r="3" spans="1:22" s="20" customFormat="1" ht="84">
       <c r="B3" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="20">
         <v>1</v>
       </c>
       <c r="F3" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>126</v>
-      </c>
-      <c r="H3" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I3" s="20" t="s">
-        <v>127</v>
       </c>
       <c r="K3" s="41">
         <v>10866</v>
       </c>
       <c r="L3" s="41"/>
       <c r="M3" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N3" s="20">
         <v>30</v>
@@ -1741,10 +1746,10 @@
         <v>29</v>
       </c>
       <c r="P3" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="R3" s="20">
         <v>14031</v>
@@ -1758,16 +1763,16 @@
     </row>
     <row r="4" spans="1:22" s="20" customFormat="1" ht="70">
       <c r="B4" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E4" s="20">
         <v>1</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I4" s="41">
         <v>1468</v>
@@ -1778,7 +1783,7 @@
       </c>
       <c r="L4" s="41"/>
       <c r="M4" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N4" s="20">
         <v>30</v>
@@ -1787,10 +1792,10 @@
         <v>29</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
       <c r="R4" s="20">
         <v>14031</v>
@@ -1804,10 +1809,10 @@
     </row>
     <row r="5" spans="1:22" s="22" customFormat="1" ht="56">
       <c r="B5" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D5" s="22">
         <v>2</v>
@@ -1819,18 +1824,18 @@
         <v>1</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J5" s="20"/>
       <c r="K5" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L5" s="20"/>
       <c r="M5" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N5" s="23">
         <v>0</v>
@@ -1839,7 +1844,7 @@
         <v>29</v>
       </c>
       <c r="P5" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q5" s="6" t="s">
         <v>56</v>
@@ -1856,22 +1861,22 @@
     </row>
     <row r="6" spans="1:22" s="23" customFormat="1" ht="28">
       <c r="A6" s="23" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="23">
         <v>3</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="23">
         <v>2</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I6" s="43">
         <v>36012</v>
@@ -1882,7 +1887,7 @@
       </c>
       <c r="L6" s="43"/>
       <c r="M6" s="43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N6" s="23">
         <v>0</v>
@@ -1891,7 +1896,7 @@
         <v>29</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q6" s="6" t="s">
         <v>56</v>
@@ -1908,22 +1913,22 @@
     </row>
     <row r="7" spans="1:22" s="44" customFormat="1" ht="140">
       <c r="B7" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E7" s="44">
         <v>3</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="44">
         <v>2</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="43">
         <v>36012</v>
@@ -1934,7 +1939,7 @@
       </c>
       <c r="L7" s="43"/>
       <c r="M7" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N7" s="44">
         <v>0</v>
@@ -1943,7 +1948,7 @@
         <v>29</v>
       </c>
       <c r="P7" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q7" s="6" t="s">
         <v>56</v>
@@ -1958,27 +1963,27 @@
         <v>1850</v>
       </c>
       <c r="U7" s="44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1">
       <c r="B8" s="23" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="23">
         <v>3</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" s="46">
         <v>2</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I8" s="43">
         <v>36012</v>
@@ -1989,7 +1994,7 @@
       </c>
       <c r="L8" s="43"/>
       <c r="M8" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="N8" s="44">
         <v>100</v>
@@ -1998,7 +2003,7 @@
         <v>29</v>
       </c>
       <c r="P8" s="23" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Q8" s="6" t="s">
         <v>56</v>
@@ -2015,19 +2020,19 @@
     </row>
     <row r="9" spans="1:22" s="23" customFormat="1" ht="28">
       <c r="A9" s="23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B9" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>140</v>
-      </c>
-      <c r="C9" s="21" t="s">
-        <v>141</v>
       </c>
       <c r="D9" s="23">
         <v>4</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="47">
         <v>40179</v>
@@ -2038,7 +2043,7 @@
       </c>
       <c r="L9" s="47"/>
       <c r="M9" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="N9" s="42">
         <v>30</v>
@@ -2050,7 +2055,7 @@
         <v>30</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="R9" s="23">
         <v>21232</v>
@@ -2105,8 +2110,8 @@
   <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A12" activePane="bottomLeft"/>
+    <sheetView topLeftCell="J1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1360" topLeftCell="A5" activePane="bottomLeft"/>
       <selection activeCell="P1" sqref="P1:P1048576"/>
       <selection pane="bottomLeft" activeCell="R25" sqref="R25"/>
     </sheetView>
@@ -2163,22 +2168,22 @@
         <v>13</v>
       </c>
       <c r="I1" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>12</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O1" s="35" t="s">
         <v>15</v>
@@ -2202,7 +2207,7 @@
         <v>4</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="W1" s="3" t="s">
         <v>0</v>
@@ -2213,46 +2218,46 @@
         <v>6</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>123</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>124</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>27</v>
@@ -2261,22 +2266,22 @@
         <v>47</v>
       </c>
       <c r="R2" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S2" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="T2" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="U2" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="U2" s="32" t="s">
-        <v>118</v>
-      </c>
       <c r="V2" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="7" customFormat="1">
@@ -2373,7 +2378,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>8</v>
@@ -2394,7 +2399,7 @@
         <v>8</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>8</v>
@@ -2426,16 +2431,16 @@
         <v>23</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M5" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N5" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>28</v>
@@ -2447,44 +2452,44 @@
         <v>31</v>
       </c>
       <c r="V5" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="42">
       <c r="I6" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N6" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>29</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R6" s="10" t="s">
         <v>51</v>
       </c>
       <c r="V6" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="42">
       <c r="I7" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N7" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R7" s="10" t="s">
         <v>52</v>
@@ -2493,10 +2498,10 @@
     </row>
     <row r="8" spans="1:23" ht="56">
       <c r="N8" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R8" s="10" t="s">
         <v>53</v>
@@ -2505,10 +2510,10 @@
     </row>
     <row r="9" spans="1:23" ht="28">
       <c r="N9" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R9" s="10" t="s">
         <v>54</v>
@@ -2517,10 +2522,10 @@
     </row>
     <row r="10" spans="1:23" ht="28">
       <c r="N10" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="Q10" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="R10" s="10" t="s">
         <v>55</v>
@@ -2528,10 +2533,10 @@
     </row>
     <row r="11" spans="1:23">
       <c r="N11" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R11" s="10" t="s">
         <v>56</v>
@@ -2539,10 +2544,10 @@
     </row>
     <row r="12" spans="1:23" ht="42">
       <c r="N12" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="Q12" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R12" s="10" t="s">
         <v>57</v>
@@ -2550,32 +2555,32 @@
     </row>
     <row r="13" spans="1:23" ht="56">
       <c r="N13" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R13" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="28">
       <c r="N14" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q14" s="10" t="s">
         <v>35</v>
       </c>
       <c r="R14" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="N15" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q15" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R15" s="10" t="s">
         <v>60</v>
@@ -2583,10 +2588,10 @@
     </row>
     <row r="16" spans="1:23">
       <c r="N16" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q16" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R16" s="10" t="s">
         <v>58</v>
@@ -2594,10 +2599,10 @@
     </row>
     <row r="17" spans="8:18">
       <c r="N17" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Q17" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R17" s="10" t="s">
         <v>59</v>
@@ -2607,15 +2612,15 @@
       <c r="H18" s="14"/>
       <c r="N18" s="39"/>
       <c r="Q18" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R18" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="8:18">
       <c r="Q19" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R19" s="10" t="s">
         <v>32</v>
@@ -2624,55 +2629,55 @@
     <row r="20" spans="8:18">
       <c r="H20" s="15"/>
       <c r="Q20" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R20" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="8:18">
       <c r="H21" s="15"/>
       <c r="Q21" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R21" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="8:18">
       <c r="H22" s="15"/>
       <c r="Q22" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R22" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="8:18">
       <c r="H23" s="14"/>
       <c r="Q23" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R23" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="8:18">
       <c r="H24" s="14"/>
       <c r="Q24" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R24" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="8:18">
       <c r="H25" s="15"/>
       <c r="Q25" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R25" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="8:18">
@@ -2681,14 +2686,14 @@
         <v>33</v>
       </c>
       <c r="R26" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="8:18">
       <c r="H27" s="14"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="8:18">
@@ -2752,14 +2757,14 @@
       <c r="H36" s="15"/>
       <c r="Q36" s="8"/>
       <c r="R36" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="8:18">
       <c r="H37" s="15"/>
       <c r="Q37" s="8"/>
       <c r="R37" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="8:18">
@@ -3254,7 +3259,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="C2" sqref="C2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3270,13 +3275,13 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="17" t="s">
         <v>26</v>
@@ -3288,16 +3293,16 @@
         <v>16</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="28">
       <c r="A2" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="10"/>
       <c r="C2" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>28</v>
@@ -3309,41 +3314,41 @@
         <v>31</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28">
       <c r="A3" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>51</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>52</v>
@@ -3354,11 +3359,11 @@
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>53</v>
@@ -3369,11 +3374,11 @@
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>54</v>
@@ -3384,11 +3389,11 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>55</v>
@@ -3399,11 +3404,11 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>56</v>
@@ -3414,11 +3419,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
       <c r="C9" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>57</v>
@@ -3429,14 +3434,14 @@
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G10" s="10"/>
     </row>
@@ -3444,14 +3449,14 @@
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G11" s="10"/>
     </row>
@@ -3459,11 +3464,11 @@
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
       <c r="C12" s="38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D12" s="10"/>
       <c r="E12" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>60</v>
@@ -3474,11 +3479,11 @@
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>58</v>
@@ -3489,11 +3494,11 @@
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>59</v>
@@ -3506,10 +3511,10 @@
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="10"/>
     </row>
@@ -3519,7 +3524,7 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>32</v>
@@ -3532,10 +3537,10 @@
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G17" s="10"/>
     </row>
@@ -3545,10 +3550,10 @@
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="10"/>
     </row>
@@ -3558,10 +3563,10 @@
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
       <c r="E19" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G19" s="10"/>
     </row>
@@ -3571,10 +3576,10 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
       <c r="E20" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="10"/>
     </row>
@@ -3584,10 +3589,10 @@
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F21" s="10" t="s">
         <v>162</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>163</v>
       </c>
       <c r="G21" s="10"/>
     </row>
@@ -3597,10 +3602,10 @@
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
       <c r="E22" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="10"/>
     </row>
@@ -3613,7 +3618,7 @@
         <v>33</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G23" s="10"/>
     </row>
@@ -3624,7 +3629,7 @@
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
       <c r="F24" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G24" s="10"/>
     </row>
@@ -3723,7 +3728,7 @@
       <c r="D33" s="10"/>
       <c r="E33" s="10"/>
       <c r="F33" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G33" s="10"/>
     </row>
@@ -3734,7 +3739,7 @@
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G34" s="10"/>
     </row>

</xml_diff>

<commit_message>
Piv#171623460 A new version of the transfer spreadsheet template
</commit_message>
<xml_diff>
--- a/ui/app/static/transfer_template.xlsx
+++ b/ui/app/static/transfer_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mieke\Gaia\DAP QSA\Business Analysis\Transfers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\Transfer Templates for QSA Testing\Internal testing templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B478892A-29C5-45AE-8475-3584719BD74F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A23C4-5205-450A-A1FC-3A6FB83E2D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Transfer List Template" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="153">
   <si>
     <t>Remarks</t>
   </si>
@@ -471,9 +471,6 @@
   </si>
   <si>
     <t>Digital media - Optical - DVD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Photographic  - Negative </t>
   </si>
   <si>
     <t>Digital media - Floppy disk - 8"</t>
@@ -531,6 +528,27 @@
       </rPr>
       <t xml:space="preserve"> i.e. there can be multiple representations of one item. Mandatory to have either "Sequence number" or a value in "Attachment Related to a Sequence Number" that references a "Sequence Number".</t>
     </r>
+  </si>
+  <si>
+    <t>Photographic - Print</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Negative </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Transparency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photographic - Glass Plate Negative </t>
+  </si>
+  <si>
+    <t>Photographic - Slide</t>
+  </si>
+  <si>
+    <t>Canister</t>
+  </si>
+  <si>
+    <t>Box</t>
   </si>
 </sst>
 </file>
@@ -1603,37 +1621,37 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.85546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="52" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" style="56" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="56" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" style="5" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="5" customWidth="1"/>
-    <col min="13" max="13" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" style="5" customWidth="1"/>
-    <col min="22" max="22" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.85546875" style="5"/>
+    <col min="1" max="1" width="16.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.3984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="36.86328125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.86328125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="14.86328125" style="52" customWidth="1"/>
+    <col min="7" max="7" width="23.1328125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="15.86328125" style="56" customWidth="1"/>
+    <col min="9" max="9" width="15.86328125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" style="56" customWidth="1"/>
+    <col min="11" max="11" width="15.3984375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="10.265625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="8.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.265625" style="5" customWidth="1"/>
+    <col min="15" max="15" width="13.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.3984375" style="5" customWidth="1"/>
+    <col min="17" max="17" width="10.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.73046875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.86328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.86328125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="20.73046875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.86328125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="19" customFormat="1" ht="57" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
@@ -1701,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B2" s="63"/>
       <c r="C2" s="66"/>
       <c r="D2" s="13"/>
@@ -1716,7 +1734,7 @@
       <c r="N2" s="24"/>
       <c r="U2" s="5"/>
     </row>
-    <row r="3" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B3" s="63"/>
       <c r="C3" s="66"/>
       <c r="D3" s="13"/>
@@ -1730,7 +1748,7 @@
       <c r="M3" s="23"/>
       <c r="N3" s="24"/>
     </row>
-    <row r="4" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B4" s="63"/>
       <c r="C4" s="66"/>
       <c r="D4" s="13"/>
@@ -1744,7 +1762,7 @@
       <c r="M4" s="23"/>
       <c r="N4" s="24"/>
     </row>
-    <row r="5" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B5" s="63"/>
       <c r="C5" s="66"/>
       <c r="D5" s="13"/>
@@ -1758,7 +1776,7 @@
       <c r="M5" s="23"/>
       <c r="N5" s="24"/>
     </row>
-    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B6" s="67"/>
       <c r="C6" s="66"/>
       <c r="D6" s="13"/>
@@ -1772,7 +1790,7 @@
       <c r="M6" s="23"/>
       <c r="N6" s="24"/>
     </row>
-    <row r="7" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B7" s="67"/>
       <c r="C7" s="66"/>
       <c r="D7" s="13"/>
@@ -1786,7 +1804,7 @@
       <c r="M7" s="23"/>
       <c r="N7" s="24"/>
     </row>
-    <row r="8" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B8" s="67"/>
       <c r="C8" s="61"/>
       <c r="D8" s="13"/>
@@ -1800,7 +1818,7 @@
       <c r="M8" s="23"/>
       <c r="N8" s="61"/>
     </row>
-    <row r="9" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B9" s="67"/>
       <c r="C9" s="66"/>
       <c r="D9" s="13"/>
@@ -1814,7 +1832,7 @@
       <c r="M9" s="23"/>
       <c r="N9" s="24"/>
     </row>
-    <row r="10" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B10" s="68"/>
       <c r="C10" s="66"/>
       <c r="D10" s="13"/>
@@ -1828,7 +1846,7 @@
       <c r="M10" s="23"/>
       <c r="N10" s="24"/>
     </row>
-    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A11" s="8"/>
       <c r="B11" s="68"/>
       <c r="C11" s="66"/>
@@ -1845,7 +1863,7 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B12" s="67"/>
       <c r="C12" s="66"/>
       <c r="D12" s="16"/>
@@ -1866,7 +1884,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="16"/>
       <c r="B13" s="67"/>
       <c r="C13" s="66"/>
@@ -1890,7 +1908,7 @@
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
     </row>
-    <row r="14" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16"/>
       <c r="B14" s="67"/>
       <c r="C14" s="66"/>
@@ -1914,7 +1932,7 @@
       <c r="U14" s="16"/>
       <c r="V14" s="16"/>
     </row>
-    <row r="15" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="16"/>
       <c r="B15" s="67"/>
       <c r="C15" s="66"/>
@@ -1938,7 +1956,7 @@
       <c r="U15" s="16"/>
       <c r="V15" s="16"/>
     </row>
-    <row r="16" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A16" s="16"/>
       <c r="B16" s="67"/>
       <c r="C16" s="66"/>
@@ -1962,7 +1980,7 @@
       <c r="U16" s="16"/>
       <c r="V16" s="16"/>
     </row>
-    <row r="17" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="16"/>
       <c r="B17" s="63"/>
       <c r="C17" s="66"/>
@@ -1986,7 +2004,7 @@
       <c r="U17" s="16"/>
       <c r="V17" s="16"/>
     </row>
-    <row r="18" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A18" s="7"/>
       <c r="B18" s="63"/>
       <c r="C18" s="66"/>
@@ -2010,7 +2028,7 @@
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
     </row>
-    <row r="19" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B19" s="63"/>
       <c r="C19" s="66"/>
       <c r="D19" s="13"/>
@@ -2030,7 +2048,7 @@
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
     </row>
-    <row r="20" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
       <c r="B20" s="63"/>
       <c r="C20" s="66"/>
@@ -2054,7 +2072,7 @@
       <c r="U20" s="5"/>
       <c r="V20" s="5"/>
     </row>
-    <row r="21" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="16"/>
       <c r="B21" s="63"/>
       <c r="C21" s="66"/>
@@ -2078,7 +2096,7 @@
       <c r="U21" s="16"/>
       <c r="V21" s="16"/>
     </row>
-    <row r="22" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B22" s="24"/>
       <c r="C22" s="66"/>
       <c r="E22" s="13"/>
@@ -2098,7 +2116,7 @@
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
     </row>
-    <row r="23" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="B23" s="63"/>
       <c r="C23" s="66"/>
       <c r="E23" s="13"/>
@@ -2118,7 +2136,7 @@
       <c r="S23" s="7"/>
       <c r="T23" s="7"/>
     </row>
-    <row r="24" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5"/>
       <c r="B24" s="61"/>
       <c r="C24" s="66"/>
@@ -2140,7 +2158,7 @@
       <c r="U24" s="5"/>
       <c r="V24" s="5"/>
     </row>
-    <row r="25" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5"/>
       <c r="B25" s="61"/>
       <c r="C25" s="66"/>
@@ -2162,7 +2180,7 @@
       <c r="U25" s="5"/>
       <c r="V25" s="5"/>
     </row>
-    <row r="26" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="12"/>
       <c r="B26" s="61"/>
       <c r="C26" s="66"/>
@@ -2186,7 +2204,7 @@
       <c r="U26" s="12"/>
       <c r="V26" s="12"/>
     </row>
-    <row r="27" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="8"/>
       <c r="B27" s="64"/>
       <c r="C27" s="66"/>
@@ -2209,7 +2227,7 @@
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
     </row>
-    <row r="28" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5"/>
       <c r="B28" s="64"/>
       <c r="C28" s="66"/>
@@ -2233,7 +2251,7 @@
       <c r="U28" s="5"/>
       <c r="V28" s="5"/>
     </row>
-    <row r="29" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
       <c r="B29" s="64"/>
       <c r="C29" s="66"/>
@@ -2256,7 +2274,7 @@
       <c r="U29" s="5"/>
       <c r="V29" s="5"/>
     </row>
-    <row r="30" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
       <c r="B30" s="64"/>
       <c r="C30" s="66"/>
@@ -2279,7 +2297,7 @@
       <c r="U30" s="5"/>
       <c r="V30" s="5"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B31" s="64"/>
       <c r="C31" s="66"/>
       <c r="D31" s="16"/>
@@ -2300,7 +2318,7 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32" s="8"/>
       <c r="B32" s="64"/>
       <c r="C32" s="66"/>
@@ -2324,7 +2342,7 @@
       <c r="U32" s="8"/>
       <c r="V32" s="8"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A33" s="8"/>
       <c r="B33" s="64"/>
       <c r="C33" s="66"/>
@@ -2348,7 +2366,7 @@
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A34" s="8"/>
       <c r="B34" s="64"/>
       <c r="C34" s="66"/>
@@ -2372,7 +2390,7 @@
       <c r="U34" s="8"/>
       <c r="V34" s="8"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A35" s="8"/>
       <c r="B35" s="64"/>
       <c r="C35" s="66"/>
@@ -2396,7 +2414,7 @@
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A36" s="16"/>
       <c r="B36" s="64"/>
       <c r="C36" s="66"/>
@@ -2420,7 +2438,7 @@
       <c r="U36" s="16"/>
       <c r="V36" s="16"/>
     </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B37" s="64"/>
       <c r="C37" s="66"/>
       <c r="E37" s="13"/>
@@ -2435,7 +2453,7 @@
       <c r="N37" s="24"/>
       <c r="R37" s="7"/>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B38" s="64"/>
       <c r="C38" s="66"/>
       <c r="E38" s="13"/>
@@ -2450,7 +2468,7 @@
       <c r="N38" s="24"/>
       <c r="R38" s="7"/>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B39" s="64"/>
       <c r="C39" s="66"/>
       <c r="E39" s="13"/>
@@ -2477,20 +2495,20 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>INDIRECT("Rep_Type[Representation Type]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K1:K1048576 I1:I1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576 K1:K1048576" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>INDIRECT("Date_Qualifier[Date Qualifier]")</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q13:Q1048576 Q1:Q11 P1:P1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>INDIRECT("Access_Category[Access Category]")</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="O1:O1048576 H38:H1048576 H1 J1 J38:J1048576" xr:uid="{F1FBDD20-6590-40F0-919B-E0491EEB3844}"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G1:G21 G23:G1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>INDIRECT("Formats[Format]")</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N9:N1048576 N1:N7" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>INDIRECT("Contained[Contained Within]")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U39:U1048576 U1:U37" xr:uid="{00000000-0002-0000-0000-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U1:U1048576" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>INDIRECT("Sensitivity[Sensitivity Label]")</formula1>
     </dataValidation>
   </dataValidations>
@@ -2523,34 +2541,34 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" style="38" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="38" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="47.42578125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.7109375" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.42578125" style="38" customWidth="1"/>
-    <col min="11" max="12" width="16.140625" style="38" customWidth="1"/>
-    <col min="13" max="13" width="22.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" style="38" customWidth="1"/>
-    <col min="15" max="15" width="44.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.86328125" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.73046875" style="38" customWidth="1"/>
+    <col min="3" max="3" width="19.86328125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="20.3984375" style="38" customWidth="1"/>
+    <col min="5" max="5" width="47.3984375" style="38" customWidth="1"/>
+    <col min="6" max="6" width="38.86328125" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.73046875" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="45.73046875" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.3984375" style="38" customWidth="1"/>
+    <col min="11" max="12" width="16.1328125" style="38" customWidth="1"/>
+    <col min="13" max="13" width="22.265625" style="38" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.1328125" style="38" customWidth="1"/>
+    <col min="15" max="15" width="44.265625" style="38" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="23" style="38" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.42578125" style="40" customWidth="1"/>
-    <col min="18" max="18" width="26.42578125" style="38" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" style="38" customWidth="1"/>
-    <col min="20" max="20" width="31.7109375" style="38" customWidth="1"/>
-    <col min="21" max="21" width="36.28515625" style="38" customWidth="1"/>
-    <col min="22" max="22" width="40.7109375" style="38" customWidth="1"/>
-    <col min="23" max="23" width="18.42578125" style="38" customWidth="1"/>
-    <col min="24" max="25" width="8.85546875" style="41"/>
-    <col min="26" max="16384" width="8.85546875" style="38"/>
+    <col min="17" max="17" width="20.3984375" style="40" customWidth="1"/>
+    <col min="18" max="18" width="26.3984375" style="38" customWidth="1"/>
+    <col min="19" max="19" width="24.265625" style="38" customWidth="1"/>
+    <col min="20" max="20" width="31.73046875" style="38" customWidth="1"/>
+    <col min="21" max="21" width="36.265625" style="38" customWidth="1"/>
+    <col min="22" max="22" width="40.73046875" style="38" customWidth="1"/>
+    <col min="23" max="23" width="18.3984375" style="38" customWidth="1"/>
+    <col min="24" max="25" width="8.86328125" style="41"/>
+    <col min="26" max="16384" width="8.86328125" style="38"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="30" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="29" t="s">
         <v>20</v>
       </c>
@@ -2621,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="28" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="28" customFormat="1" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A2" s="27" t="s">
         <v>6</v>
       </c>
@@ -2635,10 +2653,10 @@
         <v>92</v>
       </c>
       <c r="E2" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>145</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>146</v>
       </c>
       <c r="G2" s="28" t="s">
         <v>133</v>
@@ -2692,7 +2710,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="29" t="s">
         <v>21</v>
       </c>
@@ -2763,7 +2781,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="35" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="36" t="s">
         <v>22</v>
       </c>
@@ -2834,7 +2852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="29" t="s">
         <v>23</v>
       </c>
@@ -2863,7 +2881,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="G6" s="33" t="s">
         <v>27</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="H7" s="40" t="s">
         <v>74</v>
       </c>
@@ -2910,7 +2928,7 @@
       </c>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="57" x14ac:dyDescent="0.45">
       <c r="H8" s="40" t="s">
         <v>75</v>
       </c>
@@ -2922,7 +2940,7 @@
       </c>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="H9" s="40" t="s">
         <v>76</v>
       </c>
@@ -2934,7 +2952,7 @@
       </c>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="H10" s="38" t="s">
         <v>77</v>
       </c>
@@ -2945,7 +2963,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.45">
       <c r="H11" s="38" t="s">
         <v>78</v>
       </c>
@@ -2956,7 +2974,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="H12" s="38" t="s">
         <v>79</v>
       </c>
@@ -2967,7 +2985,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="57" x14ac:dyDescent="0.45">
       <c r="H13" s="38" t="s">
         <v>80</v>
       </c>
@@ -2978,7 +2996,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="28.5" x14ac:dyDescent="0.45">
       <c r="H14" s="38" t="s">
         <v>33</v>
       </c>
@@ -2989,7 +3007,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="42.75" x14ac:dyDescent="0.45">
       <c r="H15" s="38" t="s">
         <v>81</v>
       </c>
@@ -3000,7 +3018,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="16" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.45">
       <c r="H16" s="38" t="s">
         <v>82</v>
       </c>
@@ -3011,7 +3029,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H17" s="38" t="s">
         <v>83</v>
       </c>
@@ -3022,7 +3040,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H18" s="38" t="s">
         <v>84</v>
       </c>
@@ -3034,7 +3052,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H19" s="38" t="s">
         <v>85</v>
       </c>
@@ -3042,7 +3060,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H20" s="38" t="s">
         <v>86</v>
       </c>
@@ -3051,7 +3069,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H21" s="40" t="s">
         <v>87</v>
       </c>
@@ -3060,7 +3078,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H22" s="40" t="s">
         <v>88</v>
       </c>
@@ -3069,7 +3087,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H23" s="40" t="s">
         <v>89</v>
       </c>
@@ -3078,7 +3096,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H24" s="40" t="s">
         <v>90</v>
       </c>
@@ -3087,7 +3105,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H25" s="40" t="s">
         <v>91</v>
       </c>
@@ -3096,7 +3114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H26" s="40" t="s">
         <v>31</v>
       </c>
@@ -3105,21 +3123,21 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H27" s="33"/>
       <c r="N27" s="44"/>
       <c r="O27" s="38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H28" s="33"/>
       <c r="N28" s="44"/>
       <c r="O28" s="38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H29" s="33"/>
       <c r="N29" s="45"/>
       <c r="O29" s="38" t="s">
@@ -3127,531 +3145,531 @@
       </c>
       <c r="P29" s="33"/>
     </row>
-    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H30" s="33"/>
       <c r="N30" s="45"/>
       <c r="O30" s="38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H31" s="33"/>
       <c r="N31" s="45"/>
       <c r="O31" s="38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="8:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="8:17" x14ac:dyDescent="0.45">
       <c r="H32" s="33"/>
       <c r="N32" s="45"/>
       <c r="O32" s="38" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H33" s="33"/>
       <c r="N33" s="45"/>
       <c r="O33" s="38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H34" s="33"/>
       <c r="N34" s="45"/>
       <c r="O34" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H35" s="33"/>
       <c r="N35" s="45"/>
       <c r="O35" s="38" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H36" s="33"/>
       <c r="N36" s="45"/>
       <c r="O36" s="38" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H37" s="33"/>
       <c r="N37" s="45"/>
       <c r="O37" s="38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H38" s="33"/>
       <c r="N38" s="45"/>
       <c r="O38" s="38" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H39" s="33"/>
       <c r="N39" s="45"/>
       <c r="O39" s="38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="40" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H40" s="33"/>
       <c r="N40" s="45"/>
       <c r="O40" s="38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H41" s="33"/>
       <c r="N41" s="45"/>
       <c r="O41" s="38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H42" s="33"/>
       <c r="N42" s="45"/>
       <c r="O42" s="38" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H43" s="33"/>
       <c r="N43" s="44"/>
       <c r="O43" s="33"/>
     </row>
-    <row r="44" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H44" s="33"/>
       <c r="O44" s="33"/>
     </row>
-    <row r="45" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H45" s="33"/>
       <c r="O45" s="33"/>
     </row>
-    <row r="46" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H46" s="33"/>
       <c r="O46" s="33"/>
     </row>
-    <row r="47" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H47" s="33"/>
       <c r="O47" s="33"/>
     </row>
-    <row r="48" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H48" s="33"/>
       <c r="O48" s="33"/>
     </row>
-    <row r="49" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H49" s="33"/>
       <c r="O49" s="33"/>
     </row>
-    <row r="50" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H50" s="33"/>
       <c r="O50" s="33"/>
     </row>
-    <row r="51" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H51" s="33"/>
       <c r="O51" s="33"/>
     </row>
-    <row r="52" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H52" s="33"/>
       <c r="O52" s="33"/>
     </row>
-    <row r="53" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H53" s="33"/>
       <c r="O53" s="33"/>
     </row>
-    <row r="54" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H54" s="33"/>
     </row>
-    <row r="55" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H55" s="33"/>
     </row>
-    <row r="56" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H56" s="33"/>
     </row>
-    <row r="57" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H57" s="33"/>
     </row>
-    <row r="58" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H58" s="33"/>
       <c r="O58" s="33"/>
     </row>
-    <row r="59" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H59" s="33"/>
       <c r="O59" s="33"/>
     </row>
-    <row r="60" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H60" s="33"/>
       <c r="O60" s="33"/>
     </row>
-    <row r="61" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H61" s="33"/>
       <c r="O61" s="33"/>
     </row>
-    <row r="62" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H62" s="33"/>
       <c r="O62" s="33"/>
     </row>
-    <row r="63" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H63" s="46"/>
     </row>
-    <row r="64" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H64" s="46"/>
       <c r="O64" s="34"/>
     </row>
-    <row r="65" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H65" s="46"/>
       <c r="O65" s="34"/>
     </row>
-    <row r="66" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H66" s="46"/>
       <c r="O66" s="33"/>
     </row>
-    <row r="67" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H67" s="46"/>
       <c r="O67" s="33"/>
     </row>
-    <row r="68" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H68" s="46"/>
       <c r="O68" s="33"/>
     </row>
-    <row r="69" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H69" s="46"/>
       <c r="O69" s="33"/>
     </row>
-    <row r="70" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H70" s="46"/>
       <c r="O70" s="33"/>
     </row>
-    <row r="71" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H71" s="46"/>
       <c r="O71" s="33"/>
     </row>
-    <row r="72" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H72" s="33"/>
       <c r="O72" s="33"/>
     </row>
-    <row r="73" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H73" s="33"/>
       <c r="O73" s="33"/>
     </row>
-    <row r="74" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H74" s="33"/>
       <c r="O74" s="33"/>
     </row>
-    <row r="75" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H75" s="33"/>
       <c r="O75" s="33"/>
     </row>
-    <row r="76" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H76" s="33"/>
       <c r="O76" s="33"/>
     </row>
-    <row r="77" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H77" s="33"/>
       <c r="O77" s="33"/>
     </row>
-    <row r="78" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H78" s="33"/>
       <c r="O78" s="33"/>
     </row>
-    <row r="79" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H79" s="33"/>
       <c r="O79" s="33"/>
     </row>
-    <row r="80" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H80" s="33"/>
       <c r="O80" s="33"/>
     </row>
-    <row r="81" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H81" s="33"/>
       <c r="O81" s="33"/>
     </row>
-    <row r="82" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H82" s="33"/>
       <c r="O82" s="33"/>
     </row>
-    <row r="83" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H83" s="33"/>
       <c r="O83" s="33"/>
     </row>
-    <row r="84" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H84" s="33"/>
       <c r="O84" s="33"/>
     </row>
-    <row r="85" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H85" s="33"/>
       <c r="O85" s="33"/>
     </row>
-    <row r="86" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H86" s="33"/>
       <c r="O86" s="33"/>
     </row>
-    <row r="87" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H87" s="33"/>
       <c r="O87" s="33"/>
     </row>
-    <row r="88" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H88" s="33"/>
       <c r="O88" s="33"/>
     </row>
-    <row r="89" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H89" s="33"/>
       <c r="O89" s="33"/>
     </row>
-    <row r="90" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H90" s="33"/>
       <c r="O90" s="33"/>
     </row>
-    <row r="91" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H91" s="33"/>
       <c r="O91" s="33"/>
     </row>
-    <row r="92" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H92" s="33"/>
       <c r="O92" s="33"/>
     </row>
-    <row r="93" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H93" s="33"/>
       <c r="O93" s="33"/>
     </row>
-    <row r="94" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H94" s="33"/>
       <c r="O94" s="33"/>
     </row>
-    <row r="95" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H95" s="33"/>
       <c r="O95" s="33"/>
     </row>
-    <row r="96" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H96" s="33"/>
       <c r="O96" s="33"/>
     </row>
-    <row r="97" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H97" s="33"/>
       <c r="O97" s="33"/>
     </row>
-    <row r="98" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H98" s="33"/>
       <c r="O98" s="33"/>
     </row>
-    <row r="99" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H99" s="33"/>
       <c r="O99" s="33"/>
     </row>
-    <row r="100" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H100" s="33"/>
       <c r="O100" s="33"/>
     </row>
-    <row r="101" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H101" s="33"/>
       <c r="O101" s="33"/>
     </row>
-    <row r="102" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H102" s="33"/>
       <c r="O102" s="33"/>
     </row>
-    <row r="103" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H103" s="33"/>
       <c r="O103" s="33"/>
     </row>
-    <row r="104" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H104" s="33"/>
       <c r="O104" s="33"/>
     </row>
-    <row r="105" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H105" s="33"/>
       <c r="O105" s="33"/>
     </row>
-    <row r="106" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H106" s="33"/>
       <c r="O106" s="33"/>
     </row>
-    <row r="107" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H107" s="46"/>
       <c r="O107" s="33"/>
     </row>
-    <row r="108" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H108" s="46"/>
       <c r="O108" s="33"/>
     </row>
-    <row r="109" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H109" s="33"/>
       <c r="O109" s="33"/>
     </row>
-    <row r="110" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H110" s="33"/>
       <c r="O110" s="33"/>
     </row>
-    <row r="111" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H111" s="33"/>
       <c r="O111" s="33"/>
     </row>
-    <row r="112" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H112" s="33"/>
       <c r="O112" s="33"/>
     </row>
-    <row r="113" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H113" s="33"/>
       <c r="O113" s="33"/>
     </row>
-    <row r="114" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H114" s="33"/>
       <c r="O114" s="33"/>
     </row>
-    <row r="115" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H115" s="33"/>
       <c r="O115" s="33"/>
     </row>
-    <row r="116" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H116" s="33"/>
       <c r="O116" s="33"/>
     </row>
-    <row r="117" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H117" s="33"/>
       <c r="O117" s="33"/>
     </row>
-    <row r="118" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H118" s="33"/>
       <c r="O118" s="33"/>
     </row>
-    <row r="119" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H119" s="33"/>
       <c r="O119" s="33"/>
     </row>
-    <row r="120" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H120" s="33"/>
       <c r="O120" s="33"/>
     </row>
-    <row r="121" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H121" s="33"/>
       <c r="O121" s="33"/>
     </row>
-    <row r="122" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H122" s="33"/>
       <c r="O122" s="33"/>
     </row>
-    <row r="123" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H123" s="33"/>
       <c r="O123" s="33"/>
     </row>
-    <row r="124" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H124" s="33"/>
       <c r="O124" s="33"/>
     </row>
-    <row r="125" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H125" s="33"/>
       <c r="O125" s="33"/>
     </row>
-    <row r="126" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H126" s="33"/>
       <c r="O126" s="33"/>
     </row>
-    <row r="127" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="127" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H127" s="33"/>
       <c r="O127" s="33"/>
     </row>
-    <row r="128" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="128" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H128" s="33"/>
       <c r="O128" s="33"/>
     </row>
-    <row r="129" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="129" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H129" s="33"/>
       <c r="O129" s="33"/>
     </row>
-    <row r="130" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="130" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H130" s="33"/>
       <c r="O130" s="33"/>
     </row>
-    <row r="131" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="131" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H131" s="33"/>
       <c r="O131" s="33"/>
     </row>
-    <row r="132" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="132" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H132" s="33"/>
       <c r="O132" s="33"/>
     </row>
-    <row r="133" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="133" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H133" s="33"/>
       <c r="O133" s="33"/>
     </row>
-    <row r="134" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="134" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H134" s="33"/>
       <c r="O134" s="33"/>
     </row>
-    <row r="135" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="135" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H135" s="33"/>
       <c r="O135" s="33"/>
     </row>
-    <row r="136" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="136" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H136" s="33"/>
       <c r="O136" s="33"/>
     </row>
-    <row r="137" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="137" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H137" s="33"/>
       <c r="O137" s="33"/>
     </row>
-    <row r="138" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="138" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H138" s="33"/>
       <c r="O138" s="33"/>
     </row>
-    <row r="139" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="139" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H139" s="33"/>
       <c r="O139" s="33"/>
     </row>
-    <row r="140" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="140" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H140" s="33"/>
       <c r="O140" s="33"/>
     </row>
-    <row r="141" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="141" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H141" s="33"/>
       <c r="O141" s="33"/>
     </row>
-    <row r="142" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="142" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H142" s="33"/>
       <c r="O142" s="33"/>
     </row>
-    <row r="143" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="143" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H143" s="33"/>
       <c r="O143" s="33"/>
     </row>
-    <row r="144" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="144" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H144" s="33"/>
       <c r="O144" s="33"/>
     </row>
-    <row r="145" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="145" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H145" s="33"/>
       <c r="O145" s="33"/>
     </row>
-    <row r="146" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="146" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H146" s="33"/>
       <c r="O146" s="33"/>
     </row>
-    <row r="147" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="147" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H147" s="33"/>
       <c r="O147" s="33"/>
     </row>
-    <row r="148" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="148" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H148" s="33"/>
       <c r="O148" s="33"/>
     </row>
-    <row r="149" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="149" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H149" s="33"/>
       <c r="O149" s="33"/>
     </row>
-    <row r="150" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="150" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H150" s="33"/>
     </row>
-    <row r="151" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="151" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H151" s="33"/>
     </row>
-    <row r="152" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="152" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H152" s="33"/>
     </row>
-    <row r="153" spans="8:15" x14ac:dyDescent="0.25">
+    <row r="153" spans="8:15" x14ac:dyDescent="0.45">
       <c r="H153" s="33"/>
     </row>
   </sheetData>
@@ -3674,22 +3692,20 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="69.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="62.86328125" customWidth="1"/>
     <col min="7" max="7" width="64" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="53" t="s">
         <v>112</v>
       </c>
@@ -3712,7 +3728,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="9" t="s">
@@ -3731,7 +3747,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
@@ -3754,7 +3770,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>65</v>
       </c>
@@ -3773,7 +3789,7 @@
       </c>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="9" t="s">
@@ -3788,7 +3804,7 @@
       </c>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="9" t="s">
@@ -3803,7 +3819,7 @@
       </c>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="9" t="s">
@@ -3818,7 +3834,7 @@
       </c>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="9" t="s">
@@ -3833,7 +3849,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="9" t="s">
@@ -3848,7 +3864,7 @@
       </c>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="11" t="s">
@@ -3863,7 +3879,7 @@
       </c>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="11" t="s">
@@ -3878,7 +3894,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="25" t="s">
@@ -3893,7 +3909,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="11" t="s">
@@ -3908,7 +3924,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="11" t="s">
@@ -3923,7 +3939,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="11" t="s">
@@ -3934,11 +3950,11 @@
         <v>84</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>108</v>
+        <v>152</v>
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -3951,72 +3967,72 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="59" t="s">
-        <v>86</v>
+        <v>146</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>109</v>
+        <v>151</v>
       </c>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="60" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>70</v>
       </c>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="60" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>110</v>
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="60" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>61</v>
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="60" t="s">
-        <v>90</v>
+        <v>150</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>122</v>
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4029,7 +4045,7 @@
       </c>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4042,7 +4058,7 @@
       </c>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4053,7 +4069,7 @@
       </c>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4064,7 +4080,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4075,7 +4091,7 @@
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4086,7 +4102,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4097,7 +4113,7 @@
       </c>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4108,7 +4124,7 @@
       </c>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4119,7 +4135,7 @@
       </c>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4130,7 +4146,7 @@
       </c>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4141,7 +4157,7 @@
       </c>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4152,7 +4168,7 @@
       </c>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4163,7 +4179,7 @@
       </c>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4174,40 +4190,40 @@
       </c>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>

</xml_diff>

<commit_message>
Piv#171623460 Another new version of the transfer spreadsheet template
</commit_message>
<xml_diff>
--- a/ui/app/static/transfer_template.xlsx
+++ b/ui/app/static/transfer_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megan\Desktop\Transfer Templates for QSA Testing\Internal testing templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0A23C4-5205-450A-A1FC-3A6FB83E2D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{75255DCD-068B-4772-BB8F-AAC3EB1E93AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" tabRatio="832" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Transfer List Template" sheetId="1" r:id="rId1"/>
@@ -452,9 +452,6 @@
     <t>This defines whether the Representation is Digital or Physical.</t>
   </si>
   <si>
-    <t>Vocabulary choices for how Representations are contained.</t>
-  </si>
-  <si>
     <t>Agency can indicate if the Responsible Agency is different to to the Transferring Agency. QSA will review this field to make sure a valid Responsible Agency ID (just the number, not including the prefix) is imported into ArchivesSpace.  Only relevant for Item rows.</t>
   </si>
   <si>
@@ -549,6 +546,9 @@
   </si>
   <si>
     <t>Box</t>
+  </si>
+  <si>
+    <t>Vocabulary choices for how Representations are contained.  Digital Representations must use a vocab option which contains Digital Media at the start.</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1619,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -2537,9 +2537,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2653,10 +2651,10 @@
         <v>92</v>
       </c>
       <c r="E2" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>145</v>
       </c>
       <c r="G2" s="28" t="s">
         <v>133</v>
@@ -2683,7 +2681,7 @@
         <v>116</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>132</v>
@@ -2695,16 +2693,16 @@
         <v>130</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="T2" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="U2" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="U2" s="28" t="s">
+      <c r="V2" s="28" t="s">
         <v>136</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>137</v>
       </c>
       <c r="W2" s="28" t="s">
         <v>93</v>
@@ -3950,7 +3948,7 @@
         <v>84</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G15" s="3"/>
     </row>
@@ -3973,10 +3971,10 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="59" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G17" s="3"/>
     </row>
@@ -3986,7 +3984,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="60" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>70</v>
@@ -3999,7 +3997,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>110</v>
@@ -4012,7 +4010,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="60" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>61</v>
@@ -4025,7 +4023,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="60" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>122</v>
@@ -4164,7 +4162,7 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G33" s="3"/>
     </row>
@@ -4175,7 +4173,7 @@
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G34" s="3"/>
     </row>
@@ -4197,7 +4195,7 @@
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G36" s="3"/>
     </row>
@@ -4208,7 +4206,7 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G37" s="3"/>
     </row>
@@ -4219,7 +4217,7 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G38" s="3"/>
     </row>

</xml_diff>